<commit_message>
Suppression d'images inutiles + modifications rapport d'analyse
</commit_message>
<xml_diff>
--- a/Rapport d'analyse.xlsx
+++ b/Rapport d'analyse.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Salex\OneDrive\Bureau\SELLIER_Alexandre_Projet N°4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Salex\OneDrive\Bureau\FormationDev\Projets\SELLIER_Alexandre_Projet N°4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DA80FF3-66C5-4800-80AD-E501626F8C60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{234275C1-8B8B-4618-B2F7-17FB8949728B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="159">
   <si>
     <t>Catégorie</t>
   </si>
@@ -500,6 +500,9 @@
   </si>
   <si>
     <t>Observation</t>
+  </si>
+  <si>
+    <t>Augmentation du SEO</t>
   </si>
 </sst>
 </file>
@@ -645,9 +648,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -656,6 +656,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1044,8 +1047,8 @@
   </sheetPr>
   <dimension ref="A1:Z989"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="C1" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1080,7 +1083,7 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="15" t="s">
         <v>157</v>
       </c>
       <c r="H1" s="3"/>
@@ -1104,7 +1107,7 @@
       <c r="Z1" s="3"/>
     </row>
     <row r="2" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="10"/>
@@ -1235,43 +1238,45 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="G9" s="10"/>
+      <c r="G9" s="9" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="10" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="6" t="s">
         <v>32</v>
       </c>
       <c r="G10" s="10"/>
@@ -1407,22 +1412,22 @@
       </c>
     </row>
     <row r="17" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="6" t="s">
         <v>140</v>
       </c>
       <c r="G17" s="10"/>
@@ -1479,22 +1484,22 @@
       <c r="G19" s="12"/>
     </row>
     <row r="20" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="F20" s="6" t="s">
         <v>66</v>
       </c>
       <c r="G20" s="10"/>
@@ -1518,7 +1523,7 @@
       <c r="F21" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="G21" s="13" t="s">
+      <c r="G21" s="16" t="s">
         <v>146</v>
       </c>
     </row>
@@ -1541,7 +1546,7 @@
       <c r="F22" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="G22" s="13"/>
+      <c r="G22" s="16"/>
     </row>
     <row r="23" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
@@ -1565,12 +1570,12 @@
       <c r="G23" s="10"/>
     </row>
     <row r="24" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="14"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
+      <c r="A24" s="13"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
       <c r="G24" s="10"/>
     </row>
     <row r="25" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Modification du rapport d'analyse
</commit_message>
<xml_diff>
--- a/Rapport d'analyse.xlsx
+++ b/Rapport d'analyse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Salex\OneDrive\Bureau\FormationDev\Projets\SELLIER_Alexandre_Projet N°4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{234275C1-8B8B-4618-B2F7-17FB8949728B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C75A1DC-35BE-444D-B6B2-E7A7E60208E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="155">
   <si>
     <t>Catégorie</t>
   </si>
@@ -99,21 +99,12 @@
     <t>MDN – https://developer.mozilla.org/fr/docs/Web/HTML/Element/meta/name</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Aucune description du site</t>
-  </si>
-  <si>
     <t>Ajout d’une description dans la base meta description</t>
   </si>
   <si>
     <t>MDN – https://developer.mozilla.org/fr/docs/Web/HTML/Element/meta</t>
   </si>
   <si>
-    <t>Localisation</t>
-  </si>
-  <si>
     <t>La localisation ne correspond pas aux visiteurs concernés</t>
   </si>
   <si>
@@ -178,21 +169,6 @@
   </si>
   <si>
     <t>MDN - https://developer.mozilla.org/fr/docs/Learn/Forms/Your_first_form</t>
-  </si>
-  <si>
-    <t>Liens redondants</t>
-  </si>
-  <si>
-    <t>Certains liens mènent aux même URL</t>
-  </si>
-  <si>
-    <t>Évitez la répétition dans le code pour éviter les redondances</t>
-  </si>
-  <si>
-    <t>Modifier les liens ou les fusionner</t>
-  </si>
-  <si>
-    <t>Wave Tools</t>
   </si>
   <si>
     <t>Rajouter les balises sémantique</t>
@@ -274,12 +250,6 @@
     <t>Accessibilité</t>
   </si>
   <si>
-    <t>Nom du site</t>
-  </si>
-  <si>
-    <t>Le site n’a pas de nom</t>
-  </si>
-  <si>
     <t>Mettre un nom de site correct pour le référencement et l’accessibilité</t>
   </si>
   <si>
@@ -304,12 +274,6 @@
     <t>Cours OpenClassrooms – Créez des designs visuels accessibles</t>
   </si>
   <si>
-    <t>Contraste des couleurs</t>
-  </si>
-  <si>
-    <t>Certains blocs de textes sont peu lisible</t>
-  </si>
-  <si>
     <t>Créer un contraste entre le background et le texte suffisant pour être lisible</t>
   </si>
   <si>
@@ -503,6 +467,30 @@
   </si>
   <si>
     <t>Augmentation du SEO</t>
+  </si>
+  <si>
+    <t>Aucune description</t>
+  </si>
+  <si>
+    <t>La description sert de résumé de la page</t>
+  </si>
+  <si>
+    <t>La localisation des mots-clés est mauvaise</t>
+  </si>
+  <si>
+    <t>Cela rend les pages plus lentes à chargées</t>
+  </si>
+  <si>
+    <t>Mauvais nom de site</t>
+  </si>
+  <si>
+    <t>Mauvais contraste des couleurs</t>
+  </si>
+  <si>
+    <t>Le site contient un nom qui ne correspond pas à la page et complique la  recherche</t>
+  </si>
+  <si>
+    <t>Certains blocs de textes sont peu lisible à cause du contraste</t>
   </si>
 </sst>
 </file>
@@ -1045,10 +1033,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z989"/>
+  <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1084,7 +1072,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
@@ -1131,22 +1119,22 @@
         <v>7</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>9</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1157,13 +1145,13 @@
         <v>10</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>11</v>
@@ -1190,7 +1178,7 @@
         <v>16</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1198,10 +1186,10 @@
         <v>7</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>17</v>
@@ -1228,13 +1216,13 @@
         <v>22</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>23</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1242,22 +1230,22 @@
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="F9" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>27</v>
-      </c>
       <c r="G9" s="9" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1265,19 +1253,19 @@
         <v>7</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="F10" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="G10" s="10"/>
     </row>
@@ -1286,22 +1274,22 @@
         <v>7</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>36</v>
-      </c>
       <c r="F11" s="6" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1309,19 +1297,19 @@
         <v>7</v>
       </c>
       <c r="B12" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="F12" s="7" t="s">
         <v>38</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>41</v>
       </c>
       <c r="G12" s="10"/>
     </row>
@@ -1330,19 +1318,19 @@
         <v>7</v>
       </c>
       <c r="B13" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="F13" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>45</v>
       </c>
       <c r="G13" s="10"/>
     </row>
@@ -1351,448 +1339,436 @@
         <v>7</v>
       </c>
       <c r="B14" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="F14" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="G14" s="10"/>
+    </row>
+    <row r="15" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="F15" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="F14" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="G14" s="10"/>
-    </row>
-    <row r="15" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="G15" s="10"/>
+      <c r="G15" s="6" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="16" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>136</v>
+        <v>50</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>137</v>
+        <v>51</v>
       </c>
       <c r="D16" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="G16" s="10"/>
+    </row>
+    <row r="17" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="C17" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="H17"/>
+      <c r="I17"/>
+      <c r="J17"/>
+      <c r="K17"/>
+      <c r="L17"/>
+      <c r="M17"/>
+      <c r="N17"/>
+      <c r="O17"/>
+      <c r="P17"/>
+      <c r="Q17"/>
+      <c r="R17"/>
+      <c r="S17"/>
+      <c r="T17"/>
+      <c r="U17"/>
+      <c r="V17"/>
+      <c r="W17"/>
+      <c r="X17"/>
+      <c r="Y17"/>
+      <c r="Z17"/>
+    </row>
+    <row r="18" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="12"/>
+    </row>
+    <row r="19" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="E19" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="G16" s="6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="17" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="6" t="s">
+      <c r="F19" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="G17" s="10"/>
-    </row>
-    <row r="18" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="H18"/>
-      <c r="I18"/>
-      <c r="J18"/>
-      <c r="K18"/>
-      <c r="L18"/>
-      <c r="M18"/>
-      <c r="N18"/>
-      <c r="O18"/>
-      <c r="P18"/>
-      <c r="Q18"/>
-      <c r="R18"/>
-      <c r="S18"/>
-      <c r="T18"/>
-      <c r="U18"/>
-      <c r="V18"/>
-      <c r="W18"/>
-      <c r="X18"/>
-      <c r="Y18"/>
-      <c r="Z18"/>
-    </row>
-    <row r="19" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="11"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="12"/>
+      <c r="G19" s="10"/>
     </row>
     <row r="20" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="C20" s="6" t="s">
+      <c r="F20" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="D20" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="G20" s="10"/>
+      <c r="G20" s="16" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="21" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B21" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F21" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="G21" s="16"/>
+    </row>
+    <row r="22" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="C22" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="D22" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="E22" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="G21" s="16" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="22" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" s="6" t="s">
+      <c r="F22" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="G22" s="10"/>
+    </row>
+    <row r="23" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="13"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="10"/>
+    </row>
+    <row r="24" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="B24" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="D24" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="E24" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="G22" s="16"/>
-    </row>
-    <row r="23" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="B23" s="7" t="s">
+      <c r="F24" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="G24" s="6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="C25" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="D25" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="E25" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="G23" s="10"/>
-    </row>
-    <row r="24" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="13"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="10"/>
-    </row>
-    <row r="25" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="6" t="s">
+      <c r="F25" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="G25" s="9" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D26" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="E26" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="F26" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B27" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="C27" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="D27" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="G25" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="26" spans="1:26" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B26" s="6" t="s">
+      <c r="E27" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="F27" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="D26" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="G26" s="9" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="27" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="G27" s="9" t="s">
-        <v>148</v>
-      </c>
+      <c r="G27" s="10"/>
     </row>
     <row r="28" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="G28" s="10"/>
     </row>
     <row r="29" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="F29" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>105</v>
       </c>
       <c r="G29" s="10"/>
     </row>
     <row r="30" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F30" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="F30" s="7" t="s">
-        <v>91</v>
       </c>
       <c r="G30" s="10"/>
     </row>
     <row r="31" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="F31" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>91</v>
       </c>
       <c r="G31" s="10"/>
     </row>
     <row r="32" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F32" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="F32" s="7" t="s">
-        <v>91</v>
       </c>
       <c r="G32" s="10"/>
     </row>
     <row r="33" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>91</v>
+        <v>112</v>
       </c>
       <c r="G33" s="10"/>
     </row>
-    <row r="34" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F34" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="G34" s="10"/>
+    <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
     </row>
     <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="5"/>
@@ -1848,15 +1824,7 @@
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
     </row>
-    <row r="41" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
-    </row>
+    <row r="41" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="42" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="43" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="44" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2804,10 +2772,9 @@
     <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="G20:G21"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -2816,18 +2783,18 @@
     <hyperlink ref="F9" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
     <hyperlink ref="F12" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
     <hyperlink ref="F14" r:id="rId6" display="https://developer.mozilla.org/fr/docs/Learn/Forms/Your_first_form" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="F16" r:id="rId7" display="https://fr.semrush.com/blog/balises-structurelles-html-semantique/" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="F20" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="F21" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="F23" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="F28" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="F34" r:id="rId12" display="https://developer.mozilla.org/fr/docs/Web/Accessibility/ARIA" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="F15" r:id="rId7" display="https://fr.semrush.com/blog/balises-structurelles-html-semantique/" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="F19" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="F20" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="F22" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="F27" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="F33" r:id="rId12" display="https://developer.mozilla.org/fr/docs/Web/Accessibility/ARIA" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" scale="36" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId13"/>
   <rowBreaks count="2" manualBreakCount="2">
-    <brk id="17" max="16383" man="1"/>
-    <brk id="35" max="16383" man="1"/>
+    <brk id="16" max="16383" man="1"/>
+    <brk id="34" max="16383" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>
</xml_diff>